<commit_message>
Login Smart Redirect Added. Batch and Start Date added for Export
</commit_message>
<xml_diff>
--- a/Flask/Export_File_Input_Format.xlsx
+++ b/Flask/Export_File_Input_Format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9dbbc0353ccf5299/Desktop/Admin Dashboard/Flask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC1048C2191B51F65BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A1C7BEA-28C6-4B48-809A-C19FA25006E9}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC1048C2191B51F65BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{029DB083-133A-4DB1-8052-086D4FD9C9C1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,11 +62,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,11 +348,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -376,9 +371,10 @@
     <col min="15" max="15" width="17.5703125" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
     <col min="17" max="17" width="19.85546875" customWidth="1"/>
+    <col min="18" max="19" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -396,6 +392,15 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>